<commit_message>
Commit Tarifaria Cargar Conceptos 01-07-2021 JER
-Se genero el TC CargarConceptosFijos
-Se creo el TS TarifariaTS
-Se creo el TS Collection Presentacion02-07-2021
-Se modifico el xls tarifariaxls.xls
</commit_message>
<xml_diff>
--- a/xls/tarifariaxls.xlsx
+++ b/xls/tarifariaxls.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="47">
   <si>
     <t xml:space="preserve">periodoTarifaria</t>
   </si>
@@ -113,14 +113,63 @@
   </si>
   <si>
     <t xml:space="preserve">tipo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concepto-test01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concepto-test02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concepto-test03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">350</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -188,12 +237,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -214,124 +267,318 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE1"/>
+  <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AC11" activeCellId="0" sqref="AC11"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.65234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="14.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="13.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="0" width="12.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="20.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="14.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="14.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="13.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="11.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="0" width="10.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="1" width="8.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="1" width="8.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="15.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="13" style="1" width="8.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="8.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="13.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="1" width="12.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="20.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="8.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="14.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="14.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="13.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="11.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="1" width="10.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="10.99"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="0" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="0" t="s">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="0" t="s">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="0" t="s">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="0" t="s">
+      <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="0" t="s">
+      <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="0" t="s">
+      <c r="AE1" s="1" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit Tarifaria ABM Tramites Monto 13-07-21 JER
-Se creo el TC ValidarABMTramitesMontoPE
-Se modifico el xls agregando una hoja con los conceptos y montos a
validar
-Se creo el data file TDTarifariaABMTramites
-Se creo el profile Sirt2
</commit_message>
<xml_diff>
--- a/xls/tarifariaxls.xlsx
+++ b/xls/tarifariaxls.xlsx
@@ -5,10 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Hoja3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="70">
   <si>
     <t xml:space="preserve">periodoTarifaria</t>
   </si>
@@ -124,16 +126,16 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">83</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08</t>
+    <t xml:space="preserve">22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99</t>
   </si>
   <si>
     <t xml:space="preserve">01</t>
   </si>
   <si>
-    <t xml:space="preserve">Concepto-test01</t>
+    <t xml:space="preserve">Concepto-testFijo</t>
   </si>
   <si>
     <t xml:space="preserve">150</t>
@@ -148,7 +150,7 @@
     <t xml:space="preserve">02</t>
   </si>
   <si>
-    <t xml:space="preserve">Concepto-test02</t>
+    <t xml:space="preserve">Concepto-testVariable</t>
   </si>
   <si>
     <t xml:space="preserve">250</t>
@@ -157,21 +159,91 @@
     <t xml:space="preserve">03</t>
   </si>
   <si>
-    <t xml:space="preserve">Concepto-test03</t>
+    <t xml:space="preserve">Concepto-testRegla</t>
   </si>
   <si>
     <t xml:space="preserve">350</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descripcion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Codigo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Importe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agencia Gubernamental de Control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.03.19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$6,515.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.03.27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$23,270.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.18.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$1,275.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.03.23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$18,620.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.03.26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$3,732.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.18.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$645.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Permiso de Ingreso al Microcentro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14.03.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$2,435.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14.03.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14.04.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$3,390.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14.04.02</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="[$$-2C0A]#,##0.00;[RED]\([$$-2C0A]#,##0.00\)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -193,6 +265,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -237,7 +316,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -247,6 +326,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -269,11 +356,11 @@
   </sheetPr>
   <dimension ref="A1:AE4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.65234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.37"/>
@@ -281,8 +368,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="1" width="8.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="15.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="21.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="19.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="13" style="1" width="8.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="15.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="8.46"/>
@@ -590,4 +677,191 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.62"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>